<commit_message>
fixed categories Book and Books
</commit_message>
<xml_diff>
--- a/data/filtered_amazon.xlsx
+++ b/data/filtered_amazon.xlsx
@@ -1740,7 +1740,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Book</t>
+          <t>Books</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2300,7 +2300,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Book</t>
+          <t>Books</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2860,7 +2860,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Book</t>
+          <t>Books</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">

</xml_diff>

<commit_message>
fixed the outliers + reorganisation of the code
</commit_message>
<xml_diff>
--- a/data/filtered_amazon.xlsx
+++ b/data/filtered_amazon.xlsx
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>429.7435897435897</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17">
@@ -2630,7 +2630,7 @@
         </is>
       </c>
       <c r="N39" t="n">
-        <v>429.7435897435897</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40">

</xml_diff>